<commit_message>
Done sourceSets {         main {             jniLibs.srcDirs = ['src/main/jniLibs']         }     }
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Horari.xlsx
+++ b/app/src/main/assets/Horari.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abel1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\LaSalle\DAM2\Roura\M8_Android_Studio\NCA_Fichar_hores\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E0F02DE-1E1F-44F1-B34D-F1FFE41844CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DABB8B-5BA9-416D-9EB9-E806E0D73C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2FF897B5-BEE3-4876-9502-DEEFA6D577A5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2FF897B5-BEE3-4876-9502-DEEFA6D577A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Llegeix be el excel
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Horari.xlsx
+++ b/app/src/main/assets/Horari.xlsx
@@ -8,28 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\LaSalle\DAM2\Roura\M8_Android_Studio\NCA_Fichar_hores\app\src\main\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41DABB8B-5BA9-416D-9EB9-E806E0D73C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A24A72-141D-408C-9F89-25DD068C9CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2FF897B5-BEE3-4876-9502-DEEFA6D577A5}"/>
+    <workbookView xWindow="-28920" yWindow="1965" windowWidth="29040" windowHeight="15720" xr2:uid="{2FF897B5-BEE3-4876-9502-DEEFA6D577A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -457,7 +446,7 @@
   <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,6 +578,9 @@
       <c r="E9" t="s">
         <v>21</v>
       </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -648,9 +640,6 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>